<commit_message>
modify tables to display exponentiated coefficients
</commit_message>
<xml_diff>
--- a/results/n_litigate2_menbreg.xlsx
+++ b/results/n_litigate2_menbreg.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander.jakubow/yale/projects/state-lawsuits/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3428608A-7008-2F47-8624-A1D84A95AF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861DB791-7BF6-6C48-94FC-8ADF5642DE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="21940" yWindow="500" windowWidth="12080" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="53">
   <si>
     <t>Mixed-Effects menbreg Regressions of Litigation Counts (n_litigate2)</t>
   </si>
@@ -64,180 +64,42 @@
     <t>judicial_fte_share</t>
   </si>
   <si>
-    <t>0.177</t>
-  </si>
-  <si>
-    <t>0.101</t>
-  </si>
-  <si>
-    <t>(0.152)</t>
-  </si>
-  <si>
-    <t>(0.144)</t>
-  </si>
-  <si>
     <t>judicial_pay_share</t>
   </si>
   <si>
-    <t>-0.093</t>
-  </si>
-  <si>
-    <t>-0.019</t>
-  </si>
-  <si>
-    <t>(0.146)</t>
-  </si>
-  <si>
     <t>dem_presXnominate</t>
   </si>
   <si>
-    <t>0.084***</t>
-  </si>
-  <si>
-    <t>(0.006)</t>
-  </si>
-  <si>
     <t>circXnominate</t>
   </si>
   <si>
-    <t>0.000</t>
-  </si>
-  <si>
-    <t>(0.000)</t>
-  </si>
-  <si>
     <t>dem_pres</t>
   </si>
   <si>
-    <t>-1.955***</t>
-  </si>
-  <si>
-    <t>-1.961***</t>
-  </si>
-  <si>
-    <t>(0.345)</t>
-  </si>
-  <si>
-    <t>(0.346)</t>
-  </si>
-  <si>
     <t>nominate_p50_cngr</t>
   </si>
   <si>
-    <t>-0.044***</t>
-  </si>
-  <si>
-    <t>-0.041***</t>
-  </si>
-  <si>
-    <t>(0.010)</t>
-  </si>
-  <si>
-    <t>(0.009)</t>
-  </si>
-  <si>
     <t>ag_higher_office</t>
   </si>
   <si>
-    <t>0.001</t>
-  </si>
-  <si>
-    <t>0.002</t>
-  </si>
-  <si>
-    <t>(0.003)</t>
-  </si>
-  <si>
     <t>ln_ag_tenure</t>
   </si>
   <si>
-    <t>-0.081</t>
-  </si>
-  <si>
-    <t>0.171</t>
-  </si>
-  <si>
-    <t>(0.235)</t>
-  </si>
-  <si>
-    <t>(0.163)</t>
-  </si>
-  <si>
     <t>ln_sg_experience</t>
   </si>
   <si>
-    <t>0.095</t>
-  </si>
-  <si>
-    <t>0.031</t>
-  </si>
-  <si>
-    <t>(0.200)</t>
-  </si>
-  <si>
-    <t>(0.184)</t>
-  </si>
-  <si>
     <t>sg_t14_grad</t>
   </si>
   <si>
-    <t>0.003</t>
-  </si>
-  <si>
     <t>sg_clerk_scotus</t>
   </si>
   <si>
-    <t>0.007**</t>
-  </si>
-  <si>
-    <t>0.004</t>
-  </si>
-  <si>
     <t>sg_clerk_dc</t>
   </si>
   <si>
-    <t>-0.011**</t>
-  </si>
-  <si>
-    <t>-0.007</t>
-  </si>
-  <si>
-    <t>(0.005)</t>
-  </si>
-  <si>
     <t>ln_pop_total</t>
   </si>
   <si>
-    <t>0.183*</t>
-  </si>
-  <si>
-    <t>0.167*</t>
-  </si>
-  <si>
-    <t>0.166</t>
-  </si>
-  <si>
-    <t>0.026</t>
-  </si>
-  <si>
-    <t>0.051</t>
-  </si>
-  <si>
-    <t>(0.105)</t>
-  </si>
-  <si>
-    <t>(0.089)</t>
-  </si>
-  <si>
-    <t>(0.103)</t>
-  </si>
-  <si>
-    <t>(0.100)</t>
-  </si>
-  <si>
-    <t>(0.121)</t>
-  </si>
-  <si>
     <t>Wald Chi^2</t>
   </si>
   <si>
@@ -290,12 +152,39 @@
   </si>
   <si>
     <t>*** p&lt;0.01, ** p&lt;0.05, * p&lt;0.1</t>
+  </si>
+  <si>
+    <t>1.201*</t>
+  </si>
+  <si>
+    <t>1.088***</t>
+  </si>
+  <si>
+    <t>0.142***</t>
+  </si>
+  <si>
+    <t>0.957***</t>
+  </si>
+  <si>
+    <t>1.182*</t>
+  </si>
+  <si>
+    <t>1.007**</t>
+  </si>
+  <si>
+    <t>0.989**</t>
+  </si>
+  <si>
+    <t>0.141***</t>
+  </si>
+  <si>
+    <t>0.960***</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -795,22 +684,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1185,11 +1072,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1227,22 +1114,22 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1267,633 +1154,553 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4">
+        <v>1.194</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.1060000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4">
+        <v>-0.18099999999999999</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>-0.159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="B8" s="4">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.98099999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4">
+        <v>-0.13300000000000001</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>-0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>-4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4">
+        <v>-8.9999999999999993E-3</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4">
+        <v>-8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1.1859999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4">
+        <v>-0.217</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>-0.193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4">
+        <v>1.099</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1.032</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4">
+        <v>-0.22</v>
+      </c>
+      <c r="F23" s="4">
+        <v>-0.19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1.0029999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="F25" s="4">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1.004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="F27" s="4">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0.99299999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="F29" s="4">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B30" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1.181</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="F30" s="4">
+        <v>1.052</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="4">
+        <v>-0.126</v>
+      </c>
+      <c r="C31" s="4">
+        <v>-0.105</v>
+      </c>
+      <c r="D31" s="4">
+        <v>-0.122</v>
+      </c>
+      <c r="E31" s="4">
+        <v>-0.10299999999999999</v>
+      </c>
+      <c r="F31" s="4">
+        <v>-0.127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="5" t="s">
+      <c r="E33" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="5" t="s">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="C34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="5" t="s">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="C36" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="D36" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="5" t="s">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>43</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>